<commit_message>
add package_list fix qa errors, update footer
</commit_message>
<xml_diff>
--- a/docs/argo-adap-questionnaireresponse.xlsx
+++ b/docs/argo-adap-questionnaireresponse.xlsx
@@ -742,10 +742,10 @@
     <t>ElementDefinition - details for the item</t>
   </si>
   <si>
-    <t>A reference to an [ElementDefinition](elementdefinition.html) that provides the details for the item.</t>
-  </si>
-  <si>
-    <t>The ElementDefinition must be in a [StructureDefinition](structuredefinition.html) or a [DataElement](dataelement.html), and must have a fragment identifier that identifies the specific data element by its id (Element.id). E.g. http://hl7.org/fhir/StructureDefinition/Observation#Observation.value[x].
+    <t>A reference to an [ElementDefinition](http://hl7.org/fhir/STU3/elementdefinition.html) that provides the details for the item.</t>
+  </si>
+  <si>
+    <t>The ElementDefinition must be in a [StructureDefinition](http://hl7.org/fhir/STU3/structuredefinition.html) or a [DataElement](http://hl7.org/fhir/STU3/dataelement.html), and must have a fragment identifier that identifies the specific data element by its id (Element.id). E.g. http://hl7.org/fhir/StructureDefinition/Observation#Observation.value[x].
 There is no need for this element if the item pointed to by the linkId has a definition listed.</t>
   </si>
   <si>

</xml_diff>